<commit_message>
docs: Add TIA-Screenshots to the docu for the 'SofwareUnits', 'Typed Libraries' and 'HW from Excel' examples (#58)
</commit_message>
<xml_diff>
--- a/MAC_use_cases/AdditionalContent/HardwareGenerationExcelBased.xlsx
+++ b/MAC_use_cases/AdditionalContent/HardwareGenerationExcelBased.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\01_Openness\_repos\modular-application-creator-use-cases\MAC_use_cases\AdditionalContent\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D27859D3-BEBB-4A46-B965-A5EAAB52980F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AEE319F-976A-4A7A-BAE3-B36CE5EF13CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="7275" windowWidth="29040" windowHeight="15840" xr2:uid="{800D0B12-4BC3-4B93-959A-9515D8436ED2}"/>
+    <workbookView xWindow="6930" yWindow="0" windowWidth="28800" windowHeight="15435" xr2:uid="{800D0B12-4BC3-4B93-959A-9515D8436ED2}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -152,9 +152,6 @@
     <t>Name_10</t>
   </si>
   <si>
-    <t>Name_11</t>
-  </si>
-  <si>
     <t>DeviceName_6</t>
   </si>
   <si>
@@ -170,10 +167,13 @@
     <t>DeviceName_10</t>
   </si>
   <si>
-    <t>DeviceName_11</t>
-  </si>
-  <si>
-    <t>DeviceName_12</t>
+    <t>Name_4</t>
+  </si>
+  <si>
+    <t>DeviceName_1</t>
+  </si>
+  <si>
+    <t>DeviceName_5</t>
   </si>
 </sst>
 </file>
@@ -554,8 +554,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F62A318C-456C-4897-8973-853EA103A784}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -595,7 +595,7 @@
         <v>16</v>
       </c>
       <c r="E2" t="s">
-        <v>17</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -612,7 +612,7 @@
         <v>32</v>
       </c>
       <c r="E3" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -629,7 +629,7 @@
         <v>8</v>
       </c>
       <c r="E4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -643,10 +643,10 @@
         <v>7</v>
       </c>
       <c r="D5" t="s">
-        <v>9</v>
+        <v>43</v>
       </c>
       <c r="E5" t="s">
-        <v>39</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -660,10 +660,10 @@
         <v>22</v>
       </c>
       <c r="D6" t="s">
-        <v>33</v>
+        <v>9</v>
       </c>
       <c r="E6" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -677,10 +677,10 @@
         <v>23</v>
       </c>
       <c r="D7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E7" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -694,10 +694,10 @@
         <v>6</v>
       </c>
       <c r="D8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E8" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -711,10 +711,10 @@
         <v>26</v>
       </c>
       <c r="D9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E9" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -725,10 +725,10 @@
         <v>29</v>
       </c>
       <c r="D10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E10" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -739,10 +739,10 @@
         <v>31</v>
       </c>
       <c r="D11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E11" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>